<commit_message>
Merged changes for requesting other agents release their users
</commit_message>
<xml_diff>
--- a/emma/documentation/Insert Multi Rows.xlsx
+++ b/emma/documentation/Insert Multi Rows.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="116">
   <si>
     <t>2016-04-11 09:00:00</t>
   </si>
@@ -368,6 +368,12 @@
   </si>
   <si>
     <t>ken@ken.com</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>tester@tester.com</t>
   </si>
 </sst>
 </file>
@@ -2438,10 +2444,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K12"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2518,7 +2524,7 @@
         <v>77</v>
       </c>
       <c r="J2" t="str">
-        <f t="shared" ref="J2:J12" si="0">"INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ("</f>
+        <f t="shared" ref="J2:J13" si="0">"INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ("</f>
         <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (</v>
       </c>
       <c r="K2" t="str">
@@ -2894,6 +2900,43 @@
       <c r="K12" t="str">
         <f t="shared" si="2"/>
         <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (12,NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS6','John',NULL,'0498745638',NULL,1,'2016-04-01');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" ref="K13" si="3">J13 &amp; A13 &amp; ",'" &amp; B13 &amp; "'," &amp; C13 &amp; ",'" &amp; D13 &amp; "','" &amp; E13 &amp; "'," &amp; F13 &amp; "," &amp; G13 &amp; "," &amp; H13 &amp; ",'" &amp; I13 &amp; "');"</f>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (13,'tester',NULL,'Tester','tester@tester.com',NULL,NULL,0,'2016-04-04');</v>
       </c>
     </row>
   </sheetData>
@@ -2903,6 +2946,7 @@
     <hyperlink ref="E3" r:id="rId3"/>
     <hyperlink ref="E5" r:id="rId4"/>
     <hyperlink ref="E4" r:id="rId5"/>
+    <hyperlink ref="E13" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Get push notification working, make sure new queries are assigned if existing assigned queries
</commit_message>
<xml_diff>
--- a/emma/documentation/Insert Multi Rows.xlsx
+++ b/emma/documentation/Insert Multi Rows.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="query" sheetId="1" r:id="rId1"/>
     <sheet name="user" sheetId="6" r:id="rId2"/>
     <sheet name="sample questions" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="122">
   <si>
     <t>2016-04-11 09:00:00</t>
   </si>
@@ -374,12 +374,30 @@
   </si>
   <si>
     <t>tester@tester.com</t>
+  </si>
+  <si>
+    <t>agent1</t>
+  </si>
+  <si>
+    <t>agent2</t>
+  </si>
+  <si>
+    <t>agent3</t>
+  </si>
+  <si>
+    <t>agent4</t>
+  </si>
+  <si>
+    <t>agent5</t>
+  </si>
+  <si>
+    <t>agent6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -705,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,8 +746,8 @@
       <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1">
-        <v>6</v>
+      <c r="B1" t="s">
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -749,8 +767,8 @@
       <c r="H1" t="s">
         <v>75</v>
       </c>
-      <c r="I1">
-        <v>1</v>
+      <c r="I1" t="s">
+        <v>116</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>59</v>
@@ -763,16 +781,16 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M1" t="str">
-        <f>L1 &amp; A1 &amp; "," &amp; B1 &amp; ",'" &amp; C1 &amp; "','" &amp; D1 &amp; "','" &amp; E1 &amp; "','" &amp; F1 &amp; "','" &amp; G1 &amp; "','" &amp; H1 &amp; "'," &amp; I1 &amp; ",'" &amp; J1 &amp; "'," &amp; K1 &amp; ");"</f>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (1,6,'2016-04-11 09:00:00','-33.7687822,150.904814','how tall is michael jordan','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','1.98m',1,'2016-04-11 09:10:20',2);</v>
+        <f>L1 &amp; A1 &amp; ",'" &amp; B1 &amp; "','" &amp; C1 &amp; "','" &amp; D1 &amp; "','" &amp; E1 &amp; "','" &amp; F1 &amp; "','" &amp; G1 &amp; "','" &amp; H1 &amp; "','" &amp; I1 &amp; "','" &amp; J1 &amp; "'," &amp; K1 &amp; ");"</f>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (1,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','2016-04-11 09:00:00','-33.7687822,150.904814','how tall is michael jordan','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','1.98m','agent1','2016-04-11 09:10:20',2);</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>6</v>
+      <c r="B2" t="s">
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>17</v>
@@ -792,8 +810,8 @@
       <c r="H2" t="s">
         <v>74</v>
       </c>
-      <c r="I2">
-        <v>1</v>
+      <c r="I2" t="s">
+        <v>116</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>60</v>
@@ -806,16 +824,16 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M2" t="str">
-        <f t="shared" ref="M2:M4" si="1">L2 &amp; A2 &amp; "," &amp; B2 &amp; ",'" &amp; C2 &amp; "','" &amp; D2 &amp; "','" &amp; E2 &amp; "','" &amp; F2 &amp; "','" &amp; G2 &amp; "','" &amp; H2 &amp; "'," &amp; I2 &amp; ",'" &amp; J2 &amp; "'," &amp; K2 &amp; ");"</f>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (2,6,'2016-04-11 09:05:01','-33.7687822,150.904815','how tall is barack obama','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','1.85m',1,'2016-04-11 09:10:21',2);</v>
+        <f t="shared" ref="M2:M4" si="1">L2 &amp; A2 &amp; ",'" &amp; B2 &amp; "','" &amp; C2 &amp; "','" &amp; D2 &amp; "','" &amp; E2 &amp; "','" &amp; F2 &amp; "','" &amp; G2 &amp; "','" &amp; H2 &amp; "','" &amp; I2 &amp; "','" &amp; J2 &amp; "'," &amp; K2 &amp; ");"</f>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (2,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','2016-04-11 09:05:01','-33.7687822,150.904815','how tall is barack obama','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','1.85m','agent1','2016-04-11 09:10:21',2);</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>6</v>
+      <c r="B3" t="s">
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>18</v>
@@ -835,8 +853,8 @@
       <c r="H3" t="s">
         <v>76</v>
       </c>
-      <c r="I3">
-        <v>1</v>
+      <c r="I3" t="s">
+        <v>116</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>61</v>
@@ -850,15 +868,15 @@
       </c>
       <c r="M3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (3,6,'2016-04-11 09:10:02','-33.7687822,150.904816','how old is hillary clinton','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','68 years',1,'2016-04-11 09:10:22',2);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (3,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','2016-04-11 09:10:02','-33.7687822,150.904816','how old is hillary clinton','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','68 years','agent1','2016-04-11 09:10:22',2);</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>6</v>
+      <c r="B4" t="s">
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>42</v>
@@ -878,8 +896,8 @@
       <c r="H4" t="s">
         <v>73</v>
       </c>
-      <c r="I4">
-        <v>1</v>
+      <c r="I4" t="s">
+        <v>116</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>62</v>
@@ -893,15 +911,15 @@
       </c>
       <c r="M4" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (4,6,'2016-04-11 09:10:03','-33.7687822,150.904814','how tall is napolean bonaparte','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','1.69m',1,'2016-04-11 09:10:23',2);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (4,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','2016-04-11 09:10:03','-33.7687822,150.904814','how tall is napolean bonaparte','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg','1.69m','agent1','2016-04-11 09:10:23',2);</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>6</v>
+      <c r="B5" t="s">
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>43</v>
@@ -935,16 +953,16 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M5" t="str">
-        <f>L5 &amp; A5 &amp; "," &amp; B5 &amp; ",'" &amp; C5 &amp; "','" &amp; D5 &amp; "','" &amp; E5 &amp; "','" &amp; F5 &amp; "','" &amp; G5 &amp; "'," &amp; H5 &amp; "," &amp; I5 &amp; "," &amp; J5 &amp; "," &amp; K5 &amp; ");"</f>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (5,6,'2016-04-11 09:10:04','-33.7687822,150.904814','how tall is buzz aldrin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <f>L5 &amp; A5 &amp; ",'" &amp; B5 &amp; "','" &amp; C5 &amp; "','" &amp; D5 &amp; "','" &amp; E5 &amp; "','" &amp; F5 &amp; "','" &amp; G5 &amp; "'," &amp; H5 &amp; "," &amp; I5 &amp; "," &amp; J5 &amp; "," &amp; K5 &amp; ");"</f>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (5,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','2016-04-11 09:10:04','-33.7687822,150.904814','how tall is buzz aldrin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>6</v>
+      <c r="B6" t="s">
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>44</v>
@@ -978,16 +996,16 @@
         <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (</v>
       </c>
       <c r="M6" t="str">
-        <f t="shared" ref="M6:M38" si="2">L6 &amp; A6 &amp; "," &amp; B6 &amp; ",'" &amp; C6 &amp; "','" &amp; D6 &amp; "','" &amp; E6 &amp; "','" &amp; F6 &amp; "','" &amp; G6 &amp; "'," &amp; H6 &amp; "," &amp; I6 &amp; "," &amp; J6 &amp; "," &amp; K6 &amp; ");"</f>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (6,6,'2016-04-11 09:10:05','-33.7687822,150.904814','how tall is adolf hitler','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <f t="shared" ref="M6:M38" si="2">L6 &amp; A6 &amp; ",'" &amp; B6 &amp; "','" &amp; C6 &amp; "','" &amp; D6 &amp; "','" &amp; E6 &amp; "','" &amp; F6 &amp; "','" &amp; G6 &amp; "'," &amp; H6 &amp; "," &amp; I6 &amp; "," &amp; J6 &amp; "," &amp; K6 &amp; ");"</f>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (6,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','2016-04-11 09:10:05','-33.7687822,150.904814','how tall is adolf hitler','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
-      <c r="B7">
-        <v>6</v>
+      <c r="B7" t="s">
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>45</v>
@@ -1022,15 +1040,15 @@
       </c>
       <c r="M7" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (7,6,'2016-04-11 09:10:06','-33.7687822,150.904814','how tall is stalin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (7,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','2016-04-11 09:10:06','-33.7687822,150.904814','how tall is stalin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
-      <c r="B8">
-        <v>6</v>
+      <c r="B8" t="s">
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>46</v>
@@ -1065,15 +1083,15 @@
       </c>
       <c r="M8" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (8,6,'2016-04-11 09:10:07','-33.7687822,150.904814','how tall is shaquille oneal','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (8,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','2016-04-11 09:10:07','-33.7687822,150.904814','how tall is shaquille oneal','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
-      <c r="B9">
-        <v>6</v>
+      <c r="B9" t="s">
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>47</v>
@@ -1108,15 +1126,15 @@
       </c>
       <c r="M9" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (9,6,'2016-04-11 09:10:08','-33.7687822,150.904814','how tall is bill clinton','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (9,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','2016-04-11 09:10:08','-33.7687822,150.904814','how tall is bill clinton','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
-      <c r="B10">
-        <v>6</v>
+      <c r="B10" t="s">
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>48</v>
@@ -1151,15 +1169,15 @@
       </c>
       <c r="M10" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (10,6,'2016-04-11 09:10:09','-33.7687822,150.904814','how tall is michelle obama','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (10,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','2016-04-11 09:10:09','-33.7687822,150.904814','how tall is michelle obama','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
-      <c r="B11">
-        <v>6</v>
+      <c r="B11" t="s">
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>49</v>
@@ -1194,15 +1212,15 @@
       </c>
       <c r="M11" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (11,6,'2016-04-11 09:10:10','-33.7687822,150.904814','How far is my closest train station?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (11,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','2016-04-11 09:10:10','-33.7687822,150.904814','How far is my closest train station?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
-      <c r="B12">
-        <v>6</v>
+      <c r="B12" t="s">
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>50</v>
@@ -1237,15 +1255,15 @@
       </c>
       <c r="M12" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (12,6,'2016-04-11 09:10:11','-33.7687822,150.904814','When does the next train to the city come?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (12,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','2016-04-11 09:10:11','-33.7687822,150.904814','When does the next train to the city come?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
-      <c r="B13">
-        <v>6</v>
+      <c r="B13" t="s">
+        <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>51</v>
@@ -1280,15 +1298,15 @@
       </c>
       <c r="M13" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (13,6,'2016-04-11 09:10:12','-33.7687822,150.904814','How long will it take me to walk there?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (13,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','2016-04-11 09:10:12','-33.7687822,150.904814','How long will it take me to walk there?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
-      <c r="B14">
-        <v>6</v>
+      <c r="B14" t="s">
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>52</v>
@@ -1323,15 +1341,15 @@
       </c>
       <c r="M14" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (14,6,'2016-04-11 09:10:13','-33.7687822,150.904814','What time does the train get to Melbourne Central?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (14,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','2016-04-11 09:10:13','-33.7687822,150.904814','What time does the train get to Melbourne Central?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
-      <c r="B15">
-        <v>6</v>
+      <c r="B15" t="s">
+        <v>22</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>53</v>
@@ -1366,15 +1384,15 @@
       </c>
       <c r="M15" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (15,6,'2016-04-11 09:10:14','-33.7687822,150.904814','Are there any screenings of Batman vs Superman tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (15,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','2016-04-11 09:10:14','-33.7687822,150.904814','Are there any screenings of Batman vs Superman tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
-      <c r="B16">
-        <v>6</v>
+      <c r="B16" t="s">
+        <v>22</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>54</v>
@@ -1409,15 +1427,15 @@
       </c>
       <c r="M16" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (16,6,'2016-04-11 09:10:15','-33.7687822,150.904814','Can you please book 2 tickets for me?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (16,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','2016-04-11 09:10:15','-33.7687822,150.904814','Can you please book 2 tickets for me?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
-      <c r="B17">
-        <v>6</v>
+      <c r="B17" t="s">
+        <v>22</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>55</v>
@@ -1452,15 +1470,15 @@
       </c>
       <c r="M17" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (17,6,'2016-04-11 09:10:16','-33.7687822,150.904814','Where is a good place to have Japanese food for dinner nearby?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (17,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','2016-04-11 09:10:16','-33.7687822,150.904814','Where is a good place to have Japanese food for dinner nearby?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
-      <c r="B18">
-        <v>6</v>
+      <c r="B18" t="s">
+        <v>22</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>56</v>
@@ -1495,15 +1513,15 @@
       </c>
       <c r="M18" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (18,6,'2016-04-11 09:10:17','-33.7687822,150.904814','Can you make a reservation for me before the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (18,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','2016-04-11 09:10:17','-33.7687822,150.904814','Can you make a reservation for me before the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
-      <c r="B19">
-        <v>6</v>
+      <c r="B19" t="s">
+        <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>57</v>
@@ -1538,15 +1556,15 @@
       </c>
       <c r="M19" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (19,6,'2016-04-11 09:10:18','-33.7687822,150.904814','What time does Myer close tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (19,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','2016-04-11 09:10:18','-33.7687822,150.904814','What time does Myer close tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
-      <c r="B20">
-        <v>6</v>
+      <c r="B20" t="s">
+        <v>22</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>58</v>
@@ -1581,15 +1599,15 @@
       </c>
       <c r="M20" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (20,6,'2016-04-11 09:10:19','-33.7687822,150.904814','Should I bring an umbrella?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (20,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','2016-04-11 09:10:19','-33.7687822,150.904814','Should I bring an umbrella?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>21</v>
       </c>
-      <c r="B21">
-        <v>6</v>
+      <c r="B21" t="s">
+        <v>22</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>59</v>
@@ -1624,15 +1642,15 @@
       </c>
       <c r="M21" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (21,6,'2016-04-11 09:10:20','-33.7687822,150.904814','Anything else to do in the city after the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (21,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','2016-04-11 09:10:20','-33.7687822,150.904814','Anything else to do in the city after the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>23</v>
       </c>
-      <c r="B22">
-        <v>7</v>
+      <c r="B22" t="s">
+        <v>27</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>78</v>
@@ -1667,15 +1685,15 @@
       </c>
       <c r="M22" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (23,7,'2016-04-11 08:10:04','-33.7687822,150.904814','how tall is buzz aldrin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (23,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS1','2016-04-11 08:10:04','-33.7687822,150.904814','how tall is buzz aldrin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>24</v>
       </c>
-      <c r="B23">
-        <v>7</v>
+      <c r="B23" t="s">
+        <v>27</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>79</v>
@@ -1710,15 +1728,15 @@
       </c>
       <c r="M23" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (24,7,'2016-04-11 08:10:05','-33.7687822,150.904814','how tall is adolf hitler','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (24,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS1','2016-04-11 08:10:05','-33.7687822,150.904814','how tall is adolf hitler','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>25</v>
       </c>
-      <c r="B24">
-        <v>7</v>
+      <c r="B24" t="s">
+        <v>27</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>80</v>
@@ -1753,15 +1771,15 @@
       </c>
       <c r="M24" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (25,7,'2016-04-11 08:10:06','-33.7687822,150.904814','how tall is stalin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (25,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS1','2016-04-11 08:10:06','-33.7687822,150.904814','how tall is stalin','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>26</v>
       </c>
-      <c r="B25">
-        <v>7</v>
+      <c r="B25" t="s">
+        <v>27</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>81</v>
@@ -1796,15 +1814,15 @@
       </c>
       <c r="M25" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (26,7,'2016-04-11 08:10:07','-33.7687822,150.904814','how tall is shaquille oneal','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (26,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS1','2016-04-11 08:10:07','-33.7687822,150.904814','how tall is shaquille oneal','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>27</v>
       </c>
-      <c r="B26">
-        <v>7</v>
+      <c r="B26" t="s">
+        <v>27</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>82</v>
@@ -1839,15 +1857,15 @@
       </c>
       <c r="M26" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (27,7,'2016-04-11 08:10:08','-33.7687822,150.904814','how tall is bill clinton','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (27,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS1','2016-04-11 08:10:08','-33.7687822,150.904814','how tall is bill clinton','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>28</v>
       </c>
-      <c r="B27">
-        <v>7</v>
+      <c r="B27" t="s">
+        <v>27</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>83</v>
@@ -1882,15 +1900,15 @@
       </c>
       <c r="M27" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (28,7,'2016-04-11 08:10:09','-33.7687822,150.904814','how tall is michelle obama','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (28,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS1','2016-04-11 08:10:09','-33.7687822,150.904814','how tall is michelle obama','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>30</v>
       </c>
-      <c r="B28">
-        <v>8</v>
+      <c r="B28" t="s">
+        <v>28</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>84</v>
@@ -1925,15 +1943,15 @@
       </c>
       <c r="M28" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (30,8,'2016-04-11 07:10:10','-33.7687822,150.904814','How far is my closest train station?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (30,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS2','2016-04-11 07:10:10','-33.7687822,150.904814','How far is my closest train station?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>31</v>
       </c>
-      <c r="B29">
-        <v>8</v>
+      <c r="B29" t="s">
+        <v>28</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>85</v>
@@ -1968,15 +1986,15 @@
       </c>
       <c r="M29" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (31,8,'2016-04-11 07:10:11','-33.7687822,150.904814','When does the next train to the city come?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (31,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS2','2016-04-11 07:10:11','-33.7687822,150.904814','When does the next train to the city come?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>32</v>
       </c>
-      <c r="B30">
-        <v>8</v>
+      <c r="B30" t="s">
+        <v>28</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>86</v>
@@ -2011,15 +2029,15 @@
       </c>
       <c r="M30" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (32,8,'2016-04-11 07:10:12','-33.7687822,150.904814','How long will it take me to walk there?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (32,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS2','2016-04-11 07:10:12','-33.7687822,150.904814','How long will it take me to walk there?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>33</v>
       </c>
-      <c r="B31">
-        <v>8</v>
+      <c r="B31" t="s">
+        <v>28</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>87</v>
@@ -2054,15 +2072,15 @@
       </c>
       <c r="M31" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (33,8,'2016-04-11 07:10:13','-33.7687822,150.904814','What time does the train get to Melbourne Central?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (33,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS2','2016-04-11 07:10:13','-33.7687822,150.904814','What time does the train get to Melbourne Central?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>34</v>
       </c>
-      <c r="B32">
-        <v>8</v>
+      <c r="B32" t="s">
+        <v>28</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>88</v>
@@ -2097,15 +2115,15 @@
       </c>
       <c r="M32" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (34,8,'2016-04-11 07:10:14','-33.7687822,150.904814','Are there any screenings of Batman vs Superman tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (34,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS2','2016-04-11 07:10:14','-33.7687822,150.904814','Are there any screenings of Batman vs Superman tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>35</v>
       </c>
-      <c r="B33">
-        <v>8</v>
+      <c r="B33" t="s">
+        <v>28</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>89</v>
@@ -2140,15 +2158,15 @@
       </c>
       <c r="M33" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (35,8,'2016-04-11 07:10:15','-33.7687822,150.904814','Can you please book 2 tickets for me?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (35,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS2','2016-04-11 07:10:15','-33.7687822,150.904814','Can you please book 2 tickets for me?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>37</v>
       </c>
-      <c r="B34">
-        <v>9</v>
+      <c r="B34" t="s">
+        <v>29</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>90</v>
@@ -2183,15 +2201,15 @@
       </c>
       <c r="M34" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (37,9,'2016-04-11 06:10:16','-33.7687822,150.904814','Where is a good place to have Japanese food for dinner nearby?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (37,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS3','2016-04-11 06:10:16','-33.7687822,150.904814','Where is a good place to have Japanese food for dinner nearby?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>38</v>
       </c>
-      <c r="B35">
-        <v>9</v>
+      <c r="B35" t="s">
+        <v>29</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>91</v>
@@ -2226,15 +2244,15 @@
       </c>
       <c r="M35" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (38,9,'2016-04-11 06:10:17','-33.7687822,150.904814','Can you make a reservation for me before the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (38,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS3','2016-04-11 06:10:17','-33.7687822,150.904814','Can you make a reservation for me before the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>39</v>
       </c>
-      <c r="B36">
-        <v>9</v>
+      <c r="B36" t="s">
+        <v>29</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>92</v>
@@ -2269,15 +2287,15 @@
       </c>
       <c r="M36" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (39,9,'2016-04-11 06:10:18','-33.7687822,150.904814','What time does Myer close tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (39,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS3','2016-04-11 06:10:18','-33.7687822,150.904814','What time does Myer close tonight?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>40</v>
       </c>
-      <c r="B37">
-        <v>9</v>
+      <c r="B37" t="s">
+        <v>29</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>93</v>
@@ -2312,15 +2330,15 @@
       </c>
       <c r="M37" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (40,9,'2016-04-11 06:10:19','-33.7687822,150.904814','Should I bring an umbrella?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (40,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS3','2016-04-11 06:10:19','-33.7687822,150.904814','Should I bring an umbrella?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>41</v>
       </c>
-      <c r="B38">
-        <v>9</v>
+      <c r="B38" t="s">
+        <v>29</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>94</v>
@@ -2355,7 +2373,7 @@
       </c>
       <c r="M38" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (41,9,'2016-04-11 06:10:20','-33.7687822,150.904814','Anything else to do in the city after the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
+        <v>INSERT INTO query (queryid, userid, time, location, content, audio, image, answer, assignedto, answertime, status) VALUES (41,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS3','2016-04-11 06:10:20','-33.7687822,150.904814','Anything else to do in the city after the movie?','http://www.soundjay.com/misc/bell-ringing-01.mp3','http://cdn-img.instyle.com/sites/default/files/styles/428xflex/public/images/2011/gallery/011112-Keira-Knightley-400_0.jpg',NULL,NULL,NULL,0);</v>
       </c>
     </row>
   </sheetData>
@@ -2446,8 +2464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2459,8 +2477,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>116</v>
       </c>
       <c r="B1" t="s">
         <v>21</v>
@@ -2487,17 +2505,17 @@
         <v>77</v>
       </c>
       <c r="J1" t="str">
-        <f>"INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ("</f>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (</v>
+        <f>"INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('"</f>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K1" t="str">
-        <f>J1 &amp; A1 &amp; ",'" &amp; B1 &amp; "'," &amp; C1 &amp; ",'" &amp; D1 &amp; "','" &amp; E1 &amp; "'," &amp; F1 &amp; "," &amp; G1 &amp; "," &amp; H1 &amp; ",'" &amp; I1 &amp; "');"</f>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (1,'tester',NULL,'Sanjeev','sanjeev@sanjeev.com',NULL,NULL,0,'2016-04-01');</v>
+        <f>J1 &amp; A1 &amp; "','" &amp; B1 &amp; "'," &amp; C1 &amp; ",'" &amp; D1 &amp; "','" &amp; E1 &amp; "'," &amp; F1 &amp; "," &amp; G1 &amp; "," &amp; H1 &amp; ",'" &amp; I1 &amp; "');"</f>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('agent1','tester',NULL,'Sanjeev','sanjeev@sanjeev.com',NULL,NULL,0,'2016-04-01');</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
+      <c r="A2" t="s">
+        <v>117</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
@@ -2524,17 +2542,17 @@
         <v>77</v>
       </c>
       <c r="J2" t="str">
-        <f t="shared" ref="J2:J13" si="0">"INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ("</f>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (</v>
+        <f t="shared" ref="J2:J5" si="0">"INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('"</f>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K2" t="str">
-        <f>J2 &amp; A2 &amp; ",'" &amp; B2 &amp; "'," &amp; C2 &amp; ",'" &amp; D2 &amp; "','" &amp; E2 &amp; "'," &amp; F2 &amp; "," &amp; G2 &amp; "," &amp; H2 &amp; ",'" &amp; I2 &amp; "');"</f>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (2,'tester',NULL,'Albert','albert@albert.com',NULL,NULL,0,'2016-04-01');</v>
+        <f t="shared" ref="K2:K5" si="1">J2 &amp; A2 &amp; "','" &amp; B2 &amp; "'," &amp; C2 &amp; ",'" &amp; D2 &amp; "','" &amp; E2 &amp; "'," &amp; F2 &amp; "," &amp; G2 &amp; "," &amp; H2 &amp; ",'" &amp; I2 &amp; "');"</f>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('agent2','tester',NULL,'Albert','albert@albert.com',NULL,NULL,0,'2016-04-01');</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
+      <c r="A3" t="s">
+        <v>118</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
@@ -2562,16 +2580,16 @@
       </c>
       <c r="J3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (</v>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K5" si="1">J3 &amp; A3 &amp; ",'" &amp; B3 &amp; "'," &amp; C3 &amp; ",'" &amp; D3 &amp; "','" &amp; E3 &amp; "'," &amp; F3 &amp; "," &amp; G3 &amp; "," &amp; H3 &amp; ",'" &amp; I3 &amp; "');"</f>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (3,'tester',NULL,'Amos','amos@amos.com',NULL,NULL,0,'2016-04-02');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('agent3','tester',NULL,'Amos','amos@amos.com',NULL,NULL,0,'2016-04-02');</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
+      <c r="A4" t="s">
+        <v>119</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -2599,16 +2617,16 @@
       </c>
       <c r="J4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (</v>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (4,'tester',NULL,'Ryan','ryan@ryan.com',NULL,NULL,0,'2016-04-03');</v>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('agent4','tester',NULL,'Ryan','ryan@ryan.com',NULL,NULL,0,'2016-04-03');</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
+      <c r="A5" t="s">
+        <v>120</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -2636,16 +2654,16 @@
       </c>
       <c r="J5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (</v>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (5,'tester',NULL,'Ken','ken@ken.com',NULL,NULL,0,'2016-04-04');</v>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('agent5','tester',NULL,'Ken','ken@ken.com',NULL,NULL,0,'2016-04-04');</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
+      <c r="A6" t="s">
+        <v>22</v>
       </c>
       <c r="B6" t="s">
         <v>19</v>
@@ -2672,17 +2690,17 @@
         <v>100</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (</v>
+        <f>"INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('"</f>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K6" t="str">
-        <f>J6 &amp; A6 &amp; "," &amp; B6 &amp; ",'" &amp; C6 &amp; "','" &amp; D6 &amp; "'," &amp; E6 &amp; ",'" &amp; F6 &amp; "'," &amp; G6 &amp; "," &amp; H6 &amp; ",'" &amp; I6 &amp; "');"</f>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (6,NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','Amos',NULL,'0498745632',NULL,1,'2016-04-09');</v>
+        <f>J6 &amp; A6 &amp; "'," &amp; B6 &amp; ",'" &amp; C6 &amp; "','" &amp; D6 &amp; "'," &amp; E6 &amp; ",'" &amp; F6 &amp; "'," &amp; G6 &amp; "," &amp; H6 &amp; ",'" &amp; I6 &amp; "');"</f>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu',NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzSu','Amos',NULL,'0498745632',NULL,1,'2016-04-09');</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>7</v>
+      <c r="A7" t="s">
+        <v>27</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
@@ -2709,17 +2727,17 @@
         <v>37</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (</v>
+        <f t="shared" ref="J7:J12" si="2">"INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('"</f>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" ref="K7:K12" si="2">J7 &amp; A7 &amp; "," &amp; B7 &amp; ",'" &amp; C7 &amp; "','" &amp; D7 &amp; "'," &amp; E7 &amp; ",'" &amp; F7 &amp; "'," &amp; G7 &amp; "," &amp; H7 &amp; ",'" &amp; I7 &amp; "');"</f>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (7,NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS1','Josh',NULL,'0498745633',NULL,1,'2016-04-10');</v>
+        <f t="shared" ref="K7:K12" si="3">J7 &amp; A7 &amp; "'," &amp; B7 &amp; ",'" &amp; C7 &amp; "','" &amp; D7 &amp; "'," &amp; E7 &amp; ",'" &amp; F7 &amp; "'," &amp; G7 &amp; "," &amp; H7 &amp; ",'" &amp; I7 &amp; "');"</f>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS1',NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS1','Josh',NULL,'0498745633',NULL,1,'2016-04-10');</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>8</v>
+      <c r="A8" t="s">
+        <v>28</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -2746,17 +2764,17 @@
         <v>38</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (8,NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS2','Mary',NULL,'0498745634',NULL,1,'2016-04-11');</v>
+        <f t="shared" si="3"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS2',NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS2','Mary',NULL,'0498745634',NULL,1,'2016-04-11');</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>9</v>
+      <c r="A9" t="s">
+        <v>29</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
@@ -2783,17 +2801,17 @@
         <v>39</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (9,NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS3','Bob',NULL,'0498745635',NULL,1,'2016-04-12');</v>
+        <f t="shared" si="3"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS3',NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS3','Bob',NULL,'0498745635',NULL,1,'2016-04-12');</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>10</v>
+      <c r="A10" t="s">
+        <v>30</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
@@ -2820,17 +2838,17 @@
         <v>40</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (10,NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS4','Jack',NULL,'0498745636',NULL,1,'2016-04-13');</v>
+        <f t="shared" si="3"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS4',NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS4','Jack',NULL,'0498745636',NULL,1,'2016-04-13');</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>11</v>
+      <c r="A11" t="s">
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -2857,17 +2875,17 @@
         <v>41</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (11,NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS5','Juliet',NULL,'0498745637',NULL,1,'2016-04-14');</v>
+        <f t="shared" si="3"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS5',NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS5','Juliet',NULL,'0498745637',NULL,1,'2016-04-14');</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>12</v>
+      <c r="A12" t="s">
+        <v>101</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
@@ -2894,17 +2912,17 @@
         <v>77</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (</v>
+        <f t="shared" si="2"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="2"/>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (12,NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS6','John',NULL,'0498745638',NULL,1,'2016-04-01');</v>
+        <f t="shared" si="3"/>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS6',NULL,'APA91bHUYXD_X2meMxOJ4JkWGyJVwv0Hy6UPvZ-5i42jLDoU3ofdEutPJspCuNDrxg-VutIHtfvDc8WSTziMxIwIh4YIZYzQiORoGG8VcV9R8azPTEXzRUkBMiKvGHXpOBJINljZyzS6','John',NULL,'0498745638',NULL,1,'2016-04-01');</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>13</v>
+      <c r="A13" t="s">
+        <v>121</v>
       </c>
       <c r="B13" t="s">
         <v>21</v>
@@ -2931,12 +2949,12 @@
         <v>99</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (</v>
+        <f>"INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('"</f>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" ref="K13" si="3">J13 &amp; A13 &amp; ",'" &amp; B13 &amp; "'," &amp; C13 &amp; ",'" &amp; D13 &amp; "','" &amp; E13 &amp; "'," &amp; F13 &amp; "," &amp; G13 &amp; "," &amp; H13 &amp; ",'" &amp; I13 &amp; "');"</f>
-        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES (13,'tester',NULL,'Tester','tester@tester.com',NULL,NULL,0,'2016-04-04');</v>
+        <f>J13 &amp; A13 &amp; "','" &amp; B13 &amp; "'," &amp; C13 &amp; ",'" &amp; D13 &amp; "','" &amp; E13 &amp; "'," &amp; F13 &amp; "," &amp; G13 &amp; "," &amp; H13 &amp; ",'" &amp; I13 &amp; "');"</f>
+        <v>INSERT INTO user (userid, password, regid, name, email, phone, dob, role, datejoined) VALUES ('agent6','tester',NULL,'Tester','tester@tester.com',NULL,NULL,0,'2016-04-04');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>